<commit_message>
Completing part of final exam
</commit_message>
<xml_diff>
--- a/Module 1 - Quiz/Module 1_Quiz Data_Stocks.xlsx
+++ b/Module 1 - Quiz/Module 1_Quiz Data_Stocks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anguyen\Documents\GitHub\stats-edx\Module 1 - Quiz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58C6AFFA-33FE-4582-91C1-C11C01AD6A96}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CAED226-DC5F-427F-B1CC-513A44AEBCCF}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19185" windowHeight="6570" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,16 +21,14 @@
     <definedName name="_xlchart.v1.1" hidden="1">stock!$C$2:$C$120</definedName>
     <definedName name="_xlchart.v1.10" hidden="1">stock!$C$1</definedName>
     <definedName name="_xlchart.v1.11" hidden="1">stock!$C$2:$C$120</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">stock!$C$1</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">stock!$C$2:$C$120</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">stock!$C$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">stock!$C$2:$C$120</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">stock!$D$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">stock!$D$2:$D$120</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">stock!$E$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">stock!$E$2:$E$120</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">stock!$F$1</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">stock!$F$2:$F$120</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">stock!$D$1</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">stock!$D$2:$D$120</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">stock!$E$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">stock!$E$2:$E$120</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">stock!$F$1</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">stock!$F$2:$F$120</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">stock!$C$1</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">stock!$C$2:$C$120</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
@@ -139,7 +137,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000%"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -183,7 +181,7 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -208,22 +206,22 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.5</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.7</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.9</cx:f>
+        <cx:f>_xlchart.v1.7</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -234,7 +232,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{2934249F-EFE3-47E3-BAA0-4E41BC169276}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.2</cx:f>
+              <cx:f>_xlchart.v1.0</cx:f>
               <cx:v>3M</cx:v>
             </cx:txData>
           </cx:tx>
@@ -247,7 +245,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{E025678E-391D-442F-AE87-BD1C05A9266C}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.4</cx:f>
+              <cx:f>_xlchart.v1.2</cx:f>
               <cx:v>GE</cx:v>
             </cx:txData>
           </cx:tx>
@@ -260,7 +258,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{FA912295-F3EB-4CA4-92AB-F3A7AF9B3016}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.6</cx:f>
+              <cx:f>_xlchart.v1.4</cx:f>
               <cx:v>IBM</cx:v>
             </cx:txData>
           </cx:tx>
@@ -273,7 +271,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{44B387C6-1622-47A6-97BB-BABD90F99656}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.8</cx:f>
+              <cx:f>_xlchart.v1.6</cx:f>
               <cx:v>Intel</cx:v>
             </cx:txData>
           </cx:tx>
@@ -303,7 +301,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.11</cx:f>
+        <cx:f>_xlchart.v1.9</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -314,7 +312,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{DC69F2D8-8CD6-41CF-B939-A635121B453A}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.10</cx:f>
+              <cx:f>_xlchart.v1.8</cx:f>
               <cx:v>3M</cx:v>
             </cx:txData>
           </cx:tx>
@@ -345,7 +343,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.13</cx:f>
+        <cx:f>_xlchart.v1.11</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -356,7 +354,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{F51DD1F2-8DBF-4CB5-B488-766B53ED790E}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.12</cx:f>
+              <cx:f>_xlchart.v1.10</cx:f>
               <cx:v>3M</cx:v>
             </cx:txData>
           </cx:tx>
@@ -2044,14 +2042,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>73</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -2088,8 +2086,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="4629150" y="9610725"/>
-              <a:ext cx="4572000" cy="2743200"/>
+              <a:off x="4705350" y="7572375"/>
+              <a:ext cx="5486400" cy="6496050"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -2122,15 +2120,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -2166,8 +2164,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="4581525" y="1628775"/>
-              <a:ext cx="4572000" cy="2743200"/>
+              <a:off x="4781550" y="3324225"/>
+              <a:ext cx="4733925" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -2245,7 +2243,7 @@
           <xdr:spPr>
             <a:xfrm>
               <a:off x="4667250" y="17649825"/>
-              <a:ext cx="4572000" cy="2743200"/>
+              <a:ext cx="4733925" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -2689,8 +2687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="Q45" sqref="Q45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2952,6 +2950,10 @@
       <c r="F9" s="1">
         <v>6.6334360526909775E-2</v>
       </c>
+      <c r="J9">
+        <f>COUNT(C2:C120)</f>
+        <v>119</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
@@ -2971,6 +2973,10 @@
       </c>
       <c r="F10" s="1">
         <v>4.0933789271071941E-2</v>
+      </c>
+      <c r="J10">
+        <f>+J9/4</f>
+        <v>29.75</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>